<commit_message>
Coding informe resúmen de cartera
</commit_message>
<xml_diff>
--- a/views/modules/informes/ERI.xlsx
+++ b/views/modules/informes/ERI.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\wis\views\modules\informes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D59861B-3D3A-44B7-93DE-FE2E626AFACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8BD7BC-5EC0-4F9B-A51B-E6BB80FBD7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Balance" sheetId="1" r:id="rId1"/>
+    <sheet name="ERI" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="ActCorriente">#REF!</definedName>
     <definedName name="ActTotalBruto">#REF!</definedName>
-    <definedName name="Año">Balance!#REF!</definedName>
-    <definedName name="AÑOINICIAL">Balance!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Balance!$A$2:$H$63</definedName>
-    <definedName name="CentroCos.">Balance!#REF!</definedName>
+    <definedName name="Año">ERI!#REF!</definedName>
+    <definedName name="AÑOINICIAL">ERI!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ERI!$A$2:$H$63</definedName>
+    <definedName name="CentroCos.">ERI!#REF!</definedName>
     <definedName name="CNT">#REF!</definedName>
     <definedName name="ConcentracEndeudam">#REF!</definedName>
     <definedName name="CorrecciónMonetaria">#REF!</definedName>
@@ -34,32 +34,32 @@
     <definedName name="MargenBruto">#REF!</definedName>
     <definedName name="MargenNeto">#REF!</definedName>
     <definedName name="MargenOperacional">#REF!</definedName>
-    <definedName name="Mes">Balance!#REF!</definedName>
-    <definedName name="MESINICIAL">Balance!#REF!</definedName>
+    <definedName name="Mes">ERI!#REF!</definedName>
+    <definedName name="MESINICIAL">ERI!#REF!</definedName>
     <definedName name="MNVentasNetas">#REF!</definedName>
     <definedName name="MOVtasNetas">#REF!</definedName>
     <definedName name="NivEndeudamiento">#REF!</definedName>
-    <definedName name="No.Empresa">Balance!#REF!</definedName>
-    <definedName name="NombMes">Balance!#REF!</definedName>
+    <definedName name="No.Empresa">ERI!#REF!</definedName>
+    <definedName name="NombMes">ERI!#REF!</definedName>
     <definedName name="PasCorriente">#REF!</definedName>
     <definedName name="PasivoCorriente">#REF!</definedName>
     <definedName name="PruebaAcida">#REF!</definedName>
     <definedName name="RazonCorriente">#REF!</definedName>
     <definedName name="RendimActivototal">#REF!</definedName>
     <definedName name="TotalAct.">#REF!</definedName>
-    <definedName name="TotalActCorriente">Balance!$C$40</definedName>
-    <definedName name="TotalActivo">Balance!#REF!</definedName>
-    <definedName name="TotalActNoCorriente">Balance!$C$51</definedName>
-    <definedName name="TotalOtrosActivos">Balance!#REF!</definedName>
+    <definedName name="TotalActCorriente">ERI!$C$40</definedName>
+    <definedName name="TotalActivo">ERI!#REF!</definedName>
+    <definedName name="TotalActNoCorriente">ERI!$C$51</definedName>
+    <definedName name="TotalOtrosActivos">ERI!#REF!</definedName>
     <definedName name="TotalPas3ros">#REF!</definedName>
-    <definedName name="TotalPasCorriente">Balance!$H$40</definedName>
-    <definedName name="TotalPasivo">Balance!$H$45</definedName>
-    <definedName name="TotalPasivoPatrimonio">Balance!#REF!</definedName>
-    <definedName name="TotalPasNoCorriente">Balance!$H$53</definedName>
+    <definedName name="TotalPasCorriente">ERI!$H$40</definedName>
+    <definedName name="TotalPasivo">ERI!$H$45</definedName>
+    <definedName name="TotalPasivoPatrimonio">ERI!#REF!</definedName>
+    <definedName name="TotalPasNoCorriente">ERI!$H$53</definedName>
     <definedName name="TotalPasTerc">#REF!</definedName>
-    <definedName name="TotalPatrimonio">Balance!$H$57</definedName>
-    <definedName name="Unid.MOneda">Balance!#REF!</definedName>
-    <definedName name="UNIDAD">Balance!$B$4</definedName>
+    <definedName name="TotalPatrimonio">ERI!$H$57</definedName>
+    <definedName name="Unid.MOneda">ERI!#REF!</definedName>
+    <definedName name="UNIDAD">ERI!$B$4</definedName>
     <definedName name="UtiildadBruta">#REF!</definedName>
     <definedName name="Utild.Operac.">#REF!</definedName>
     <definedName name="UtildNeta">#REF!</definedName>
@@ -212,6 +212,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -503,6 +504,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -535,7 +537,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -560,6 +561,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1532090</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>124924</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D2C75B0-1463-43BC-AFAC-263F3AB393EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9525" y="57150"/>
+          <a:ext cx="1522565" cy="610699"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -913,16 +980,16 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="25.5">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:8">
       <c r="C3" s="33"/>
@@ -936,36 +1003,36 @@
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="15.75">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="40"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="42"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
     </row>
     <row r="9" spans="1:8">
       <c r="C9" s="33"/>
@@ -974,28 +1041,28 @@
       <c r="C10" s="33"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="46"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="47"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="46"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="8" t="s">
@@ -1503,7 +1570,7 @@
         <v>29</v>
       </c>
       <c r="G62" s="5"/>
-      <c r="H62" s="47"/>
+      <c r="H62" s="37"/>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="31"/>
@@ -1530,6 +1597,10 @@
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="0.28000000000000003" bottom="0.31" header="0" footer="0"/>
   <pageSetup scale="72" orientation="landscape" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
+  <headerFooter alignWithMargins="0">
+    <oddFooter>&amp;RInforme generado por el palicativo WIS - &amp;"Arial,Negrita"Web Information System&amp;"Arial,Normal"
+&amp;D &amp;T</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>